<commit_message>
Update the table sheet
</commit_message>
<xml_diff>
--- a/Data_process/碳足迹/all_element_carbon.xlsx
+++ b/Data_process/碳足迹/all_element_carbon.xlsx
@@ -8567,7 +8567,7 @@
         <v>3</v>
       </c>
       <c r="AE85" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="86">
@@ -9422,7 +9422,7 @@
         <v>3</v>
       </c>
       <c r="AE94" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="95">
@@ -9802,7 +9802,7 @@
         <v>3</v>
       </c>
       <c r="AE98" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="99">
@@ -12747,7 +12747,7 @@
         <v>3</v>
       </c>
       <c r="AE129" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="130">
@@ -20727,7 +20727,7 @@
         <v>3</v>
       </c>
       <c r="AE213" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="214">
@@ -32887,7 +32887,7 @@
         <v>3</v>
       </c>
       <c r="AE341" t="n">
-        <v>216.24</v>
+        <v>0.5496</v>
       </c>
     </row>
     <row r="342">

</xml_diff>